<commit_message>
Ajuste da funcao de conciliacao, e criacao da barra de status
</commit_message>
<xml_diff>
--- a/11 - RELATÓRIOS DIÁRIOS E MENSAIS/01 - Importações Diárias/20 - Importações Nova x Gestão/Mercantil/conciliados/2024/2/Conciliado_19-02-2024.xlsx
+++ b/11 - RELATÓRIOS DIÁRIOS E MENSAIS/01 - Importações Diárias/20 - Importações Nova x Gestão/Mercantil/conciliados/2024/2/Conciliado_19-02-2024.xlsx
@@ -7257,7 +7257,7 @@
         <v>90</v>
       </c>
       <c r="O21" s="2">
-        <v>45337.67314814815</v>
+        <v>45337</v>
       </c>
       <c r="P21" t="s">
         <v>95</v>
@@ -7383,10 +7383,10 @@
         <v>783</v>
       </c>
       <c r="BP21" t="s">
-        <v>716</v>
+        <v>784</v>
       </c>
       <c r="BQ21" t="s">
-        <v>784</v>
+        <v>716</v>
       </c>
       <c r="BR21" t="s">
         <v>716</v>
@@ -7413,7 +7413,7 @@
         <v>906</v>
       </c>
       <c r="CF21">
-        <v>17</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:84">
@@ -7460,7 +7460,7 @@
         <v>90</v>
       </c>
       <c r="O22" s="2">
-        <v>45337.65060185185</v>
+        <v>45337</v>
       </c>
       <c r="P22" t="s">
         <v>99</v>
@@ -7586,10 +7586,10 @@
         <v>783</v>
       </c>
       <c r="BP22" t="s">
+        <v>716</v>
+      </c>
+      <c r="BQ22" t="s">
         <v>784</v>
-      </c>
-      <c r="BQ22" t="s">
-        <v>716</v>
       </c>
       <c r="BR22" t="s">
         <v>716</v>
@@ -7616,7 +7616,7 @@
         <v>906</v>
       </c>
       <c r="CF22">
-        <v>18</v>
+        <v>282</v>
       </c>
     </row>
     <row r="23" spans="1:84">
@@ -7663,7 +7663,7 @@
         <v>90</v>
       </c>
       <c r="O23" s="2">
-        <v>45337.64973379629</v>
+        <v>45337</v>
       </c>
       <c r="P23" t="s">
         <v>91</v>
@@ -7819,7 +7819,7 @@
         <v>906</v>
       </c>
       <c r="CF23">
-        <v>17</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:84">
@@ -7866,7 +7866,7 @@
         <v>90</v>
       </c>
       <c r="O24" s="2">
-        <v>45337.625625</v>
+        <v>45337</v>
       </c>
       <c r="P24" t="s">
         <v>91</v>
@@ -8022,7 +8022,7 @@
         <v>906</v>
       </c>
       <c r="CF24">
-        <v>18</v>
+        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:84">
@@ -8069,7 +8069,7 @@
         <v>90</v>
       </c>
       <c r="O25" s="2">
-        <v>45337.62085648148</v>
+        <v>45337</v>
       </c>
       <c r="P25" t="s">
         <v>95</v>
@@ -8225,7 +8225,7 @@
         <v>906</v>
       </c>
       <c r="CF25">
-        <v>18</v>
+        <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:84">
@@ -8272,7 +8272,7 @@
         <v>90</v>
       </c>
       <c r="O26" s="2">
-        <v>45337.6047337963</v>
+        <v>45337</v>
       </c>
       <c r="P26" t="s">
         <v>97</v>
@@ -8398,10 +8398,10 @@
         <v>783</v>
       </c>
       <c r="BP26" t="s">
-        <v>716</v>
+        <v>784</v>
       </c>
       <c r="BQ26" t="s">
-        <v>784</v>
+        <v>716</v>
       </c>
       <c r="BR26" t="s">
         <v>716</v>
@@ -8428,7 +8428,7 @@
         <v>906</v>
       </c>
       <c r="CF26">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:84">
@@ -8475,7 +8475,7 @@
         <v>90</v>
       </c>
       <c r="O27" s="2">
-        <v>45337.60232638889</v>
+        <v>45337</v>
       </c>
       <c r="P27" t="s">
         <v>100</v>
@@ -8601,10 +8601,10 @@
         <v>783</v>
       </c>
       <c r="BP27" t="s">
-        <v>716</v>
+        <v>784</v>
       </c>
       <c r="BQ27" t="s">
-        <v>784</v>
+        <v>716</v>
       </c>
       <c r="BR27" t="s">
         <v>716</v>
@@ -8631,7 +8631,7 @@
         <v>906</v>
       </c>
       <c r="CF27">
-        <v>18</v>
+        <v>282</v>
       </c>
     </row>
     <row r="28" spans="1:84">
@@ -8678,7 +8678,7 @@
         <v>90</v>
       </c>
       <c r="O28" s="2">
-        <v>45337.5990625</v>
+        <v>45337</v>
       </c>
       <c r="P28" t="s">
         <v>92</v>
@@ -8834,7 +8834,7 @@
         <v>906</v>
       </c>
       <c r="CF28">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="29" spans="1:84">
@@ -8881,7 +8881,7 @@
         <v>90</v>
       </c>
       <c r="O29" s="2">
-        <v>45337.59658564815</v>
+        <v>45337</v>
       </c>
       <c r="P29" t="s">
         <v>101</v>
@@ -9037,7 +9037,7 @@
         <v>906</v>
       </c>
       <c r="CF29">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:84">
@@ -9084,7 +9084,7 @@
         <v>90</v>
       </c>
       <c r="O30" s="2">
-        <v>45337.59409722222</v>
+        <v>45337</v>
       </c>
       <c r="P30" t="s">
         <v>94</v>
@@ -9240,7 +9240,7 @@
         <v>906</v>
       </c>
       <c r="CF30">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="31" spans="1:84">
@@ -9287,7 +9287,7 @@
         <v>90</v>
       </c>
       <c r="O31" s="2">
-        <v>45337.59341435185</v>
+        <v>45337</v>
       </c>
       <c r="P31" t="s">
         <v>101</v>
@@ -9413,10 +9413,10 @@
         <v>783</v>
       </c>
       <c r="BP31" t="s">
+        <v>716</v>
+      </c>
+      <c r="BQ31" t="s">
         <v>784</v>
-      </c>
-      <c r="BQ31" t="s">
-        <v>716</v>
       </c>
       <c r="BR31" t="s">
         <v>716</v>
@@ -9443,7 +9443,7 @@
         <v>906</v>
       </c>
       <c r="CF31">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="1:84">
@@ -9490,7 +9490,7 @@
         <v>90</v>
       </c>
       <c r="O32" s="2">
-        <v>45337.59111111111</v>
+        <v>45337</v>
       </c>
       <c r="P32" t="s">
         <v>98</v>
@@ -9646,7 +9646,7 @@
         <v>906</v>
       </c>
       <c r="CF32">
-        <v>18</v>
+        <v>282</v>
       </c>
     </row>
     <row r="33" spans="1:84">
@@ -9693,7 +9693,7 @@
         <v>90</v>
       </c>
       <c r="O33" s="2">
-        <v>45337.58278935185</v>
+        <v>45337</v>
       </c>
       <c r="P33" t="s">
         <v>98</v>
@@ -9819,10 +9819,10 @@
         <v>783</v>
       </c>
       <c r="BP33" t="s">
-        <v>716</v>
+        <v>784</v>
       </c>
       <c r="BQ33" t="s">
-        <v>784</v>
+        <v>716</v>
       </c>
       <c r="BR33" t="s">
         <v>716</v>
@@ -9849,7 +9849,7 @@
         <v>906</v>
       </c>
       <c r="CF33">
-        <v>18</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:84">
@@ -9896,7 +9896,7 @@
         <v>90</v>
       </c>
       <c r="O34" s="2">
-        <v>45337.58096064815</v>
+        <v>45337</v>
       </c>
       <c r="P34" t="s">
         <v>95</v>
@@ -10052,7 +10052,7 @@
         <v>906</v>
       </c>
       <c r="CF34">
-        <v>18</v>
+        <v>282</v>
       </c>
     </row>
     <row r="35" spans="1:84">
@@ -10099,7 +10099,7 @@
         <v>90</v>
       </c>
       <c r="O35" s="2">
-        <v>45337.57974537037</v>
+        <v>45337</v>
       </c>
       <c r="P35" t="s">
         <v>98</v>
@@ -10255,7 +10255,7 @@
         <v>906</v>
       </c>
       <c r="CF35">
-        <v>18</v>
+        <v>282</v>
       </c>
     </row>
     <row r="36" spans="1:84">
@@ -10302,7 +10302,7 @@
         <v>90</v>
       </c>
       <c r="O36" s="2">
-        <v>45337.57737268518</v>
+        <v>45337</v>
       </c>
       <c r="P36" t="s">
         <v>96</v>
@@ -10458,7 +10458,7 @@
         <v>906</v>
       </c>
       <c r="CF36">
-        <v>18</v>
+        <v>282</v>
       </c>
     </row>
     <row r="37" spans="1:84">
@@ -10505,7 +10505,7 @@
         <v>90</v>
       </c>
       <c r="O37" s="2">
-        <v>45337.55717592593</v>
+        <v>45337</v>
       </c>
       <c r="P37" t="s">
         <v>96</v>
@@ -10661,7 +10661,7 @@
         <v>906</v>
       </c>
       <c r="CF37">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="38" spans="1:84">
@@ -10708,7 +10708,7 @@
         <v>90</v>
       </c>
       <c r="O38" s="2">
-        <v>45337.55202546297</v>
+        <v>45337</v>
       </c>
       <c r="P38" t="s">
         <v>91</v>
@@ -10834,10 +10834,10 @@
         <v>783</v>
       </c>
       <c r="BP38" t="s">
+        <v>716</v>
+      </c>
+      <c r="BQ38" t="s">
         <v>784</v>
-      </c>
-      <c r="BQ38" t="s">
-        <v>716</v>
       </c>
       <c r="BR38" t="s">
         <v>716</v>
@@ -10864,7 +10864,7 @@
         <v>906</v>
       </c>
       <c r="CF38">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="39" spans="1:84">
@@ -10911,7 +10911,7 @@
         <v>90</v>
       </c>
       <c r="O39" s="2">
-        <v>45337.54519675926</v>
+        <v>45337</v>
       </c>
       <c r="P39" t="s">
         <v>97</v>
@@ -11067,7 +11067,7 @@
         <v>906</v>
       </c>
       <c r="CF39">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="40" spans="1:84">
@@ -11114,7 +11114,7 @@
         <v>90</v>
       </c>
       <c r="O40" s="2">
-        <v>45337.54206018519</v>
+        <v>45337</v>
       </c>
       <c r="P40" t="s">
         <v>96</v>
@@ -11240,10 +11240,10 @@
         <v>783</v>
       </c>
       <c r="BP40" t="s">
-        <v>716</v>
+        <v>784</v>
       </c>
       <c r="BQ40" t="s">
-        <v>784</v>
+        <v>716</v>
       </c>
       <c r="BR40" t="s">
         <v>716</v>
@@ -11270,7 +11270,7 @@
         <v>906</v>
       </c>
       <c r="CF40">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41" spans="1:84">
@@ -11317,7 +11317,7 @@
         <v>90</v>
       </c>
       <c r="O41" s="2">
-        <v>45337.53084490741</v>
+        <v>45337</v>
       </c>
       <c r="P41" t="s">
         <v>98</v>
@@ -11443,10 +11443,10 @@
         <v>783</v>
       </c>
       <c r="BP41" t="s">
+        <v>716</v>
+      </c>
+      <c r="BQ41" t="s">
         <v>784</v>
-      </c>
-      <c r="BQ41" t="s">
-        <v>716</v>
       </c>
       <c r="BR41" t="s">
         <v>716</v>
@@ -11473,7 +11473,7 @@
         <v>906</v>
       </c>
       <c r="CF41">
-        <v>18</v>
+        <v>282</v>
       </c>
     </row>
     <row r="42" spans="1:84">
@@ -11520,7 +11520,7 @@
         <v>90</v>
       </c>
       <c r="O42" s="2">
-        <v>45337.52840277777</v>
+        <v>45337</v>
       </c>
       <c r="P42" t="s">
         <v>93</v>
@@ -11676,7 +11676,7 @@
         <v>906</v>
       </c>
       <c r="CF42">
-        <v>21</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43" spans="1:84">
@@ -11723,7 +11723,7 @@
         <v>90</v>
       </c>
       <c r="O43" s="2">
-        <v>45337.52674768519</v>
+        <v>45337</v>
       </c>
       <c r="P43" t="s">
         <v>100</v>
@@ -11849,10 +11849,10 @@
         <v>783</v>
       </c>
       <c r="BP43" t="s">
+        <v>716</v>
+      </c>
+      <c r="BQ43" t="s">
         <v>784</v>
-      </c>
-      <c r="BQ43" t="s">
-        <v>716</v>
       </c>
       <c r="BR43" t="s">
         <v>716</v>
@@ -11879,7 +11879,7 @@
         <v>906</v>
       </c>
       <c r="CF43">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44" spans="1:84">
@@ -11926,7 +11926,7 @@
         <v>90</v>
       </c>
       <c r="O44" s="2">
-        <v>45337.52599537037</v>
+        <v>45337</v>
       </c>
       <c r="P44" t="s">
         <v>99</v>
@@ -12082,7 +12082,7 @@
         <v>906</v>
       </c>
       <c r="CF44">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="45" spans="1:84">
@@ -12129,7 +12129,7 @@
         <v>90</v>
       </c>
       <c r="O45" s="2">
-        <v>45337.513125</v>
+        <v>45337</v>
       </c>
       <c r="P45" t="s">
         <v>93</v>
@@ -12255,10 +12255,10 @@
         <v>783</v>
       </c>
       <c r="BP45" t="s">
-        <v>716</v>
+        <v>784</v>
       </c>
       <c r="BQ45" t="s">
-        <v>784</v>
+        <v>716</v>
       </c>
       <c r="BR45" t="s">
         <v>716</v>
@@ -12285,7 +12285,7 @@
         <v>906</v>
       </c>
       <c r="CF45">
-        <v>21</v>
+        <v>285</v>
       </c>
     </row>
     <row r="46" spans="1:84">
@@ -12332,7 +12332,7 @@
         <v>90</v>
       </c>
       <c r="O46" s="2">
-        <v>45337.50858796296</v>
+        <v>45337</v>
       </c>
       <c r="P46" t="s">
         <v>98</v>
@@ -12488,7 +12488,7 @@
         <v>906</v>
       </c>
       <c r="CF46">
-        <v>21</v>
+        <v>285</v>
       </c>
     </row>
     <row r="47" spans="1:84">
@@ -12535,7 +12535,7 @@
         <v>90</v>
       </c>
       <c r="O47" s="2">
-        <v>45337.50662037037</v>
+        <v>45337</v>
       </c>
       <c r="P47" t="s">
         <v>94</v>
@@ -12661,10 +12661,10 @@
         <v>783</v>
       </c>
       <c r="BP47" t="s">
+        <v>716</v>
+      </c>
+      <c r="BQ47" t="s">
         <v>784</v>
-      </c>
-      <c r="BQ47" t="s">
-        <v>716</v>
       </c>
       <c r="BR47" t="s">
         <v>716</v>
@@ -12691,7 +12691,7 @@
         <v>906</v>
       </c>
       <c r="CF47">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="48" spans="1:84">
@@ -12738,7 +12738,7 @@
         <v>90</v>
       </c>
       <c r="O48" s="2">
-        <v>45337.50505787037</v>
+        <v>45337</v>
       </c>
       <c r="P48" t="s">
         <v>101</v>
@@ -12864,10 +12864,10 @@
         <v>783</v>
       </c>
       <c r="BP48" t="s">
+        <v>716</v>
+      </c>
+      <c r="BQ48" t="s">
         <v>784</v>
-      </c>
-      <c r="BQ48" t="s">
-        <v>716</v>
       </c>
       <c r="BR48" t="s">
         <v>716</v>
@@ -12894,7 +12894,7 @@
         <v>906</v>
       </c>
       <c r="CF48">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="49" spans="1:84">
@@ -12941,7 +12941,7 @@
         <v>90</v>
       </c>
       <c r="O49" s="2">
-        <v>45337.50212962963</v>
+        <v>45337</v>
       </c>
       <c r="P49" t="s">
         <v>92</v>
@@ -13097,7 +13097,7 @@
         <v>906</v>
       </c>
       <c r="CF49">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="1:84">
@@ -13144,7 +13144,7 @@
         <v>90</v>
       </c>
       <c r="O50" s="2">
-        <v>45337.50121527778</v>
+        <v>45337</v>
       </c>
       <c r="P50" t="s">
         <v>92</v>
@@ -13300,7 +13300,7 @@
         <v>906</v>
       </c>
       <c r="CF50">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="51" spans="1:84">
@@ -13347,7 +13347,7 @@
         <v>90</v>
       </c>
       <c r="O51" s="2">
-        <v>45337.49582175926</v>
+        <v>45337</v>
       </c>
       <c r="P51" t="s">
         <v>94</v>
@@ -13503,7 +13503,7 @@
         <v>906</v>
       </c>
       <c r="CF51">
-        <v>21</v>
+        <v>285</v>
       </c>
     </row>
     <row r="52" spans="1:84">
@@ -13550,7 +13550,7 @@
         <v>90</v>
       </c>
       <c r="O52" s="2">
-        <v>45337.48581018519</v>
+        <v>45337</v>
       </c>
       <c r="P52" t="s">
         <v>99</v>
@@ -13706,7 +13706,7 @@
         <v>906</v>
       </c>
       <c r="CF52">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="53" spans="1:84">
@@ -13753,7 +13753,7 @@
         <v>90</v>
       </c>
       <c r="O53" s="2">
-        <v>45337.48357638889</v>
+        <v>45337</v>
       </c>
       <c r="P53" t="s">
         <v>101</v>
@@ -13879,10 +13879,10 @@
         <v>783</v>
       </c>
       <c r="BP53" t="s">
+        <v>716</v>
+      </c>
+      <c r="BQ53" t="s">
         <v>784</v>
-      </c>
-      <c r="BQ53" t="s">
-        <v>716</v>
       </c>
       <c r="BR53" t="s">
         <v>716</v>
@@ -13909,7 +13909,7 @@
         <v>906</v>
       </c>
       <c r="CF53">
-        <v>21</v>
+        <v>285</v>
       </c>
     </row>
     <row r="54" spans="1:84">
@@ -13956,7 +13956,7 @@
         <v>90</v>
       </c>
       <c r="O54" s="2">
-        <v>45337.48228009259</v>
+        <v>45337</v>
       </c>
       <c r="P54" t="s">
         <v>98</v>
@@ -14082,10 +14082,10 @@
         <v>783</v>
       </c>
       <c r="BP54" t="s">
+        <v>716</v>
+      </c>
+      <c r="BQ54" t="s">
         <v>784</v>
-      </c>
-      <c r="BQ54" t="s">
-        <v>716</v>
       </c>
       <c r="BR54" t="s">
         <v>716</v>
@@ -14112,7 +14112,7 @@
         <v>906</v>
       </c>
       <c r="CF54">
-        <v>20</v>
+        <v>284</v>
       </c>
     </row>
     <row r="55" spans="1:84">
@@ -14159,7 +14159,7 @@
         <v>90</v>
       </c>
       <c r="O55" s="2">
-        <v>45337.46805555555</v>
+        <v>45337</v>
       </c>
       <c r="P55" t="s">
         <v>101</v>
@@ -14315,7 +14315,7 @@
         <v>906</v>
       </c>
       <c r="CF55">
-        <v>22</v>
+        <v>286</v>
       </c>
     </row>
     <row r="56" spans="1:84">
@@ -14362,7 +14362,7 @@
         <v>90</v>
       </c>
       <c r="O56" s="2">
-        <v>45337.455625</v>
+        <v>45337</v>
       </c>
       <c r="P56" t="s">
         <v>91</v>
@@ -14488,10 +14488,10 @@
         <v>783</v>
       </c>
       <c r="BP56" t="s">
-        <v>716</v>
+        <v>784</v>
       </c>
       <c r="BQ56" t="s">
-        <v>784</v>
+        <v>716</v>
       </c>
       <c r="BR56" t="s">
         <v>716</v>
@@ -14518,7 +14518,7 @@
         <v>906</v>
       </c>
       <c r="CF56">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="57" spans="1:84">
@@ -14565,7 +14565,7 @@
         <v>90</v>
       </c>
       <c r="O57" s="2">
-        <v>45337.44844907407</v>
+        <v>45337</v>
       </c>
       <c r="P57" t="s">
         <v>95</v>
@@ -14691,10 +14691,10 @@
         <v>783</v>
       </c>
       <c r="BP57" t="s">
-        <v>716</v>
+        <v>784</v>
       </c>
       <c r="BQ57" t="s">
-        <v>784</v>
+        <v>716</v>
       </c>
       <c r="BR57" t="s">
         <v>716</v>
@@ -14721,7 +14721,7 @@
         <v>906</v>
       </c>
       <c r="CF57">
-        <v>22</v>
+        <v>286</v>
       </c>
     </row>
     <row r="58" spans="1:84">
@@ -14768,7 +14768,7 @@
         <v>90</v>
       </c>
       <c r="O58" s="2">
-        <v>45337.44255787037</v>
+        <v>45337</v>
       </c>
       <c r="P58" t="s">
         <v>96</v>
@@ -14924,7 +14924,7 @@
         <v>906</v>
       </c>
       <c r="CF58">
-        <v>23</v>
+        <v>287</v>
       </c>
     </row>
     <row r="59" spans="1:84">
@@ -14971,7 +14971,7 @@
         <v>90</v>
       </c>
       <c r="O59" s="2">
-        <v>45337.43726851852</v>
+        <v>45337</v>
       </c>
       <c r="P59" t="s">
         <v>99</v>
@@ -15127,7 +15127,7 @@
         <v>906</v>
       </c>
       <c r="CF59">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="60" spans="1:84">
@@ -15174,7 +15174,7 @@
         <v>90</v>
       </c>
       <c r="O60" s="2">
-        <v>45337.42807870371</v>
+        <v>45337</v>
       </c>
       <c r="P60" t="s">
         <v>99</v>
@@ -15300,10 +15300,10 @@
         <v>783</v>
       </c>
       <c r="BP60" t="s">
-        <v>716</v>
+        <v>784</v>
       </c>
       <c r="BQ60" t="s">
-        <v>784</v>
+        <v>716</v>
       </c>
       <c r="BR60" t="s">
         <v>716</v>
@@ -15330,7 +15330,7 @@
         <v>906</v>
       </c>
       <c r="CF60">
-        <v>21</v>
+        <v>285</v>
       </c>
     </row>
     <row r="61" spans="1:84">
@@ -15377,7 +15377,7 @@
         <v>90</v>
       </c>
       <c r="O61" s="2">
-        <v>45337.41504629629</v>
+        <v>45337</v>
       </c>
       <c r="P61" t="s">
         <v>93</v>
@@ -15503,10 +15503,10 @@
         <v>783</v>
       </c>
       <c r="BP61" t="s">
-        <v>716</v>
+        <v>784</v>
       </c>
       <c r="BQ61" t="s">
-        <v>784</v>
+        <v>716</v>
       </c>
       <c r="BR61" t="s">
         <v>716</v>
@@ -15533,7 +15533,7 @@
         <v>906</v>
       </c>
       <c r="CF61">
-        <v>23</v>
+        <v>287</v>
       </c>
     </row>
     <row r="62" spans="1:84">
@@ -15580,7 +15580,7 @@
         <v>90</v>
       </c>
       <c r="O62" s="2">
-        <v>45337.39458333333</v>
+        <v>45337</v>
       </c>
       <c r="P62" t="s">
         <v>91</v>
@@ -15736,7 +15736,7 @@
         <v>906</v>
       </c>
       <c r="CF62">
-        <v>24</v>
+        <v>288</v>
       </c>
     </row>
     <row r="63" spans="1:84">
@@ -15783,7 +15783,7 @@
         <v>90</v>
       </c>
       <c r="O63" s="2">
-        <v>45337.39402777778</v>
+        <v>45337</v>
       </c>
       <c r="P63" t="s">
         <v>92</v>
@@ -15939,7 +15939,7 @@
         <v>906</v>
       </c>
       <c r="CF63">
-        <v>23</v>
+        <v>287</v>
       </c>
     </row>
     <row r="64" spans="1:84">
@@ -15986,7 +15986,7 @@
         <v>90</v>
       </c>
       <c r="O64" s="2">
-        <v>45337.38871527778</v>
+        <v>45337</v>
       </c>
       <c r="P64" t="s">
         <v>101</v>
@@ -16142,7 +16142,7 @@
         <v>906</v>
       </c>
       <c r="CF64">
-        <v>24</v>
+        <v>288</v>
       </c>
     </row>
     <row r="65" spans="1:84">
@@ -16189,7 +16189,7 @@
         <v>90</v>
       </c>
       <c r="O65" s="2">
-        <v>45337.38649305556</v>
+        <v>45337</v>
       </c>
       <c r="P65" t="s">
         <v>95</v>
@@ -16315,10 +16315,10 @@
         <v>783</v>
       </c>
       <c r="BP65" t="s">
-        <v>716</v>
+        <v>784</v>
       </c>
       <c r="BQ65" t="s">
-        <v>784</v>
+        <v>716</v>
       </c>
       <c r="BR65" t="s">
         <v>716</v>
@@ -16345,7 +16345,7 @@
         <v>906</v>
       </c>
       <c r="CF65">
-        <v>23</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>